<commit_message>
Add 'OngkosKirimBeli` to product and update income statement calculation to include this in calculation.
</commit_message>
<xml_diff>
--- a/test/integration/project/data_bilyet_giro.xlsx
+++ b/test/integration/project/data_bilyet_giro.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="133">
   <si>
     <t>id</t>
   </si>
@@ -428,6 +428,9 @@
   </si>
   <si>
     <t>jumlahTukar</t>
+  </si>
+  <si>
+    <t>ongkosKirimBeli</t>
   </si>
 </sst>
 </file>
@@ -1947,10 +1950,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:P13"/>
+  <dimension ref="A1:Q13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P2" sqref="P2"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1959,17 +1962,17 @@
     <col min="2" max="2" width="14.140625" style="1" customWidth="1"/>
     <col min="3" max="3" width="8.42578125" customWidth="1"/>
     <col min="4" max="4" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.85546875" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.5703125" customWidth="1"/>
-    <col min="9" max="9" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="14.85546875" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.5703125" customWidth="1"/>
+    <col min="10" max="10" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1986,40 +1989,43 @@
         <v>102</v>
       </c>
       <c r="F1" t="s">
+        <v>132</v>
+      </c>
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>17</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>36</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>44</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>114</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>116</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>117</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>120</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>20</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>-1</v>
       </c>
@@ -2035,29 +2041,29 @@
       <c r="E2">
         <v>1100</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>37</v>
       </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
       <c r="J2">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="K2">
+        <v>-1</v>
+      </c>
+      <c r="L2">
         <v>1</v>
       </c>
-      <c r="L2">
+      <c r="M2">
         <v>3</v>
       </c>
-      <c r="N2">
+      <c r="O2">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>-2</v>
       </c>
@@ -2073,26 +2079,26 @@
       <c r="E3">
         <v>1600</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="H3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>27</v>
       </c>
-      <c r="I3">
-        <v>0</v>
-      </c>
       <c r="J3">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="K3">
+        <v>-1</v>
+      </c>
+      <c r="L3">
         <v>2</v>
       </c>
-      <c r="N3">
+      <c r="O3">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>-3</v>
       </c>
@@ -2108,26 +2114,26 @@
       <c r="E4">
         <v>1000</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="H4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>28</v>
       </c>
-      <c r="I4">
-        <v>0</v>
-      </c>
       <c r="J4">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="K4">
+        <v>-1</v>
+      </c>
+      <c r="L4">
         <v>1</v>
       </c>
-      <c r="N4">
+      <c r="O4">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>-4</v>
       </c>
@@ -2143,23 +2149,23 @@
       <c r="E5">
         <v>13100</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="H5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H5">
-        <v>0</v>
-      </c>
       <c r="I5">
         <v>0</v>
       </c>
       <c r="J5">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="K5">
+        <v>-1</v>
+      </c>
+      <c r="L5">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>-5</v>
       </c>
@@ -2175,23 +2181,23 @@
       <c r="E6">
         <v>600</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="H6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="H6">
-        <v>0</v>
-      </c>
       <c r="I6">
         <v>0</v>
       </c>
       <c r="J6">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="K6">
+        <v>-1</v>
+      </c>
+      <c r="L6">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>-6</v>
       </c>
@@ -2207,23 +2213,23 @@
       <c r="E7">
         <v>900</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="H7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="H7">
-        <v>0</v>
-      </c>
       <c r="I7">
         <v>0</v>
       </c>
       <c r="J7">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="K7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+        <v>-1</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>-7</v>
       </c>
@@ -2239,23 +2245,23 @@
       <c r="E8">
         <v>200</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="H8" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H8">
-        <v>0</v>
-      </c>
       <c r="I8">
         <v>0</v>
       </c>
       <c r="J8">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="K8">
+        <v>-1</v>
+      </c>
+      <c r="L8">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>-8</v>
       </c>
@@ -2271,23 +2277,23 @@
       <c r="E9">
         <v>500</v>
       </c>
-      <c r="G9" s="2" t="s">
+      <c r="H9" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="H9">
-        <v>0</v>
-      </c>
       <c r="I9">
         <v>0</v>
       </c>
       <c r="J9">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="K9">
+        <v>-1</v>
+      </c>
+      <c r="L9">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>-9</v>
       </c>
@@ -2303,23 +2309,23 @@
       <c r="E10">
         <v>400</v>
       </c>
-      <c r="G10" s="2" t="s">
+      <c r="H10" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="H10">
-        <v>0</v>
-      </c>
       <c r="I10">
         <v>0</v>
       </c>
       <c r="J10">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="K10">
+        <v>-1</v>
+      </c>
+      <c r="L10">
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>-10</v>
       </c>
@@ -2335,23 +2341,23 @@
       <c r="E11">
         <v>1500</v>
       </c>
-      <c r="G11" s="2" t="s">
+      <c r="H11" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="H11">
-        <v>0</v>
-      </c>
       <c r="I11">
         <v>0</v>
       </c>
       <c r="J11">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="K11">
+        <v>-1</v>
+      </c>
+      <c r="L11">
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>-11</v>
       </c>
@@ -2367,23 +2373,23 @@
       <c r="E12">
         <v>200</v>
       </c>
-      <c r="G12" s="2" t="s">
+      <c r="H12" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="H12">
+      <c r="I12">
         <v>10</v>
       </c>
-      <c r="I12">
-        <v>0</v>
-      </c>
       <c r="J12">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="K12">
+        <v>-1</v>
+      </c>
+      <c r="L12">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>-12</v>
       </c>
@@ -2399,19 +2405,19 @@
       <c r="E13">
         <v>200</v>
       </c>
-      <c r="G13" s="5" t="s">
+      <c r="H13" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="H13">
+      <c r="I13">
         <v>60</v>
       </c>
-      <c r="I13">
+      <c r="J13">
         <v>10</v>
       </c>
-      <c r="J13">
-        <v>-1</v>
-      </c>
       <c r="K13">
+        <v>-1</v>
+      </c>
+      <c r="L13">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
`PencairanPoinTukarUang` should generate cash transaction.
</commit_message>
<xml_diff>
--- a/test/integration/project/data_bilyet_giro.xlsx
+++ b/test/integration/project/data_bilyet_giro.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="390" windowWidth="14940" windowHeight="7455" tabRatio="815" activeTab="1"/>
+    <workbookView xWindow="360" yWindow="390" windowWidth="14940" windowHeight="7455" tabRatio="815" firstSheet="9" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="Satuan" sheetId="15" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="134">
   <si>
     <t>id</t>
   </si>
@@ -431,6 +431,9 @@
   </si>
   <si>
     <t>ongkosKirimBeli</t>
+  </si>
+  <si>
+    <t>poinBerlaku</t>
   </si>
 </sst>
 </file>
@@ -1293,10 +1296,10 @@
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet21"/>
-  <dimension ref="A1:R8"/>
+  <dimension ref="A1:S8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="S3" sqref="S3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1319,9 +1322,10 @@
     <col min="16" max="16" width="12" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>62</v>
       </c>
@@ -1376,8 +1380,11 @@
       <c r="R1" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>73</v>
       </c>
@@ -1406,8 +1413,11 @@
       <c r="R2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>73</v>
       </c>
@@ -1439,8 +1449,11 @@
       <c r="R3" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>81</v>
       </c>
@@ -1480,8 +1493,11 @@
       <c r="R4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>81</v>
       </c>
@@ -1515,8 +1531,11 @@
       <c r="R5" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>81</v>
       </c>
@@ -1553,8 +1572,11 @@
       <c r="R6" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>81</v>
       </c>
@@ -1591,8 +1613,11 @@
       <c r="R7" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S7" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>81</v>
       </c>
@@ -1628,6 +1653,9 @@
       </c>
       <c r="R8" t="b">
         <v>0</v>
+      </c>
+      <c r="S8" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1952,7 +1980,7 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:Q13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>

</xml_diff>